<commit_message>
Fix 2016 social srevices immigration office
</commit_message>
<xml_diff>
--- a/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתיים קליטה 2016.xlsx
+++ b/datapackage_pipelines_budgetkey/pipelines/activities/social_services/מיפוי שירותים חברתיים קליטה 2016.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Code/obudget/budgetkey-data-pipelines/datapackage_pipelines_budgetkey/pipelines/activities/social_services/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B582F0-2FB8-8640-BF07-F21E928007C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10785" windowHeight="4095"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="20860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="קליטה פתוח (2)" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'קליטה פתוח (2)'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -211,12 +217,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="#,###,"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,###,"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,7 +233,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -235,7 +241,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -256,7 +262,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -268,20 +274,20 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -290,7 +296,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -298,7 +304,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -306,21 +312,21 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -333,7 +339,7 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -347,7 +353,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -598,9 +604,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -616,9 +622,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -642,63 +645,6 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,9 +656,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -737,7 +680,7 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="13" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,7 +717,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="14" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -783,11 +726,68 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -803,7 +803,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -845,7 +845,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -878,9 +878,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,6 +930,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1088,32 +1122,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="51.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="21" style="14" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="14" customWidth="1"/>
-    <col min="7" max="9" width="8.88671875" style="7"/>
-    <col min="10" max="10" width="9.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="3.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21" style="13" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="13" customWidth="1"/>
+    <col min="7" max="9" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="41.25" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>30</v>
@@ -1131,227 +1165,228 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="55.5" customHeight="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="6">
-        <v>62634000</v>
-      </c>
-      <c r="F2" s="15">
+        <v>62634</v>
+      </c>
+      <c r="F2" s="14">
         <v>5600</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="38.25" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="6">
-        <v>6582000</v>
-      </c>
-      <c r="F3" s="15">
+        <v>6582</v>
+      </c>
+      <c r="F3" s="14">
         <v>712</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="31.5" customHeight="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="6">
-        <v>4500000</v>
-      </c>
-      <c r="F4" s="15">
+        <v>4500</v>
+      </c>
+      <c r="F4" s="14">
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="42" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="21" customFormat="1" ht="31.5" customHeight="1">
       <c r="A5" s="4"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="40">
-        <f>SUM(E2:E4)</f>
-        <v>73716000</v>
-      </c>
-      <c r="F5" s="41"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="6">
+        <v>73716</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="63"/>
+      <c r="D6" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="6">
-        <v>12000000</v>
-      </c>
-      <c r="F6" s="15">
+        <v>12000</v>
+      </c>
+      <c r="F6" s="14">
         <v>2214</v>
       </c>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="87" customHeight="1">
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="6">
-        <v>5800000</v>
-      </c>
-      <c r="F7" s="15">
+        <v>5800</v>
+      </c>
+      <c r="F7" s="14">
         <v>1010</v>
       </c>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" s="42" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45" t="s">
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" s="21" customFormat="1" ht="87" customHeight="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="40">
-        <f>SUM(E6:E7)</f>
-        <v>17800000</v>
-      </c>
-      <c r="F8" s="41"/>
-      <c r="J8" s="46"/>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="6">
+        <v>17800</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="6">
-        <v>14000000</v>
-      </c>
-      <c r="F9" s="15">
+        <v>14000</v>
+      </c>
+      <c r="F9" s="14">
         <v>2400</v>
       </c>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="19">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="29" t="s">
+      <c r="B10" s="60"/>
+      <c r="C10" s="59" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="6">
-        <v>2150000</v>
-      </c>
-      <c r="F10" s="15">
+        <v>2150</v>
+      </c>
+      <c r="F10" s="14">
         <v>90</v>
       </c>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="31.5" customHeight="1">
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E11" s="6">
-        <v>420000</v>
-      </c>
-      <c r="F11" s="15">
+        <v>420</v>
+      </c>
+      <c r="F11" s="14">
         <v>600</v>
       </c>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="19">
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="6">
-        <v>300000</v>
-      </c>
-      <c r="F12" s="15">
+        <v>300</v>
+      </c>
+      <c r="F12" s="14">
         <v>250</v>
       </c>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" ht="19">
       <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="6">
-        <v>381000</v>
-      </c>
-      <c r="F13" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" s="10" customFormat="1" ht="24">
       <c r="A14" s="4"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="50">
-        <f>SUM(E9:E13)</f>
-        <v>17251000</v>
-      </c>
-      <c r="F14" s="51"/>
-    </row>
-    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="6">
+        <v>17251</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="45" customHeight="1">
       <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="59" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1361,83 +1396,83 @@
         <v>45</v>
       </c>
       <c r="E15" s="6">
-        <v>5913200</v>
-      </c>
-      <c r="F15" s="15">
+        <v>5913.2</v>
+      </c>
+      <c r="F15" s="14">
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="34.5" customHeight="1">
       <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="29" t="s">
+      <c r="B16" s="60"/>
+      <c r="C16" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="6">
-        <v>2754120</v>
-      </c>
-      <c r="F16" s="15">
+        <v>2754.12</v>
+      </c>
+      <c r="F16" s="14">
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="24" customHeight="1">
       <c r="A17" s="4">
         <v>13</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="6">
-        <v>619000</v>
-      </c>
-      <c r="F17" s="15">
+        <v>619</v>
+      </c>
+      <c r="F17" s="14">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="30.75" customHeight="1">
       <c r="A18" s="4">
         <v>14</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="6">
-        <v>644000</v>
-      </c>
-      <c r="F18" s="15">
+        <v>644</v>
+      </c>
+      <c r="F18" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="30.75" customHeight="1">
       <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="6">
-        <v>1600000</v>
-      </c>
-      <c r="F19" s="15">
+        <v>1600</v>
+      </c>
+      <c r="F19" s="14">
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="41.25" customHeight="1">
       <c r="A20" s="4">
         <v>16</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1445,325 +1480,303 @@
         <v>46</v>
       </c>
       <c r="E20" s="6">
-        <v>300000</v>
-      </c>
-      <c r="F20" s="15">
+        <v>300</v>
+      </c>
+      <c r="F20" s="14">
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="41.25" customHeight="1">
       <c r="A21" s="4"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="50">
-        <f>SUM(E15:E20)</f>
-        <v>11830320</v>
-      </c>
-      <c r="F21" s="52"/>
-    </row>
-    <row r="22" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="6">
+        <v>11830.32</v>
+      </c>
+      <c r="F21" s="31"/>
+    </row>
+    <row r="22" spans="1:10" ht="25.5" customHeight="1">
       <c r="A22" s="4">
         <v>17</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="24"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="6">
-        <v>6800000</v>
-      </c>
-      <c r="F22" s="15">
+        <v>6800</v>
+      </c>
+      <c r="F22" s="14">
         <v>3000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="29.25" customHeight="1">
       <c r="A23" s="4">
         <v>18</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="6">
-        <v>1800000</v>
-      </c>
-      <c r="F23" s="15">
+        <v>1800</v>
+      </c>
+      <c r="F23" s="14">
         <v>700</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="29.25" customHeight="1">
       <c r="A24" s="4"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="50">
-        <f>SUM(E22:E23)</f>
-        <v>8600000</v>
-      </c>
-      <c r="F24" s="52"/>
-    </row>
-    <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="6">
+        <v>8600</v>
+      </c>
+      <c r="F24" s="31"/>
+    </row>
+    <row r="25" spans="1:10" ht="33" customHeight="1">
       <c r="A25" s="4">
         <v>19</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="24"/>
+      <c r="C25" s="54"/>
       <c r="D25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="6">
-        <v>4500000</v>
-      </c>
-      <c r="F25" s="15">
+        <v>4500</v>
+      </c>
+      <c r="F25" s="14">
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="36" customHeight="1">
       <c r="A26" s="4">
         <v>20</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="56"/>
       <c r="D26" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="6">
-        <v>3500000</v>
-      </c>
-      <c r="F26" s="15">
+        <v>3500</v>
+      </c>
+      <c r="F26" s="14">
         <v>100</v>
       </c>
-      <c r="J26" s="8">
-        <v>73716</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="54" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="53"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49" t="s">
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" s="33" customFormat="1" ht="36" customHeight="1">
+      <c r="A27" s="32"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="50">
-        <f>SUM(E25:E26)</f>
-        <v>8000000</v>
-      </c>
-      <c r="F27" s="52"/>
-      <c r="J27" s="66">
-        <v>17800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="6">
+        <v>8000</v>
+      </c>
+      <c r="F27" s="31"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="45"/>
+    </row>
+    <row r="28" spans="1:10" ht="37.5" customHeight="1">
       <c r="A28" s="4">
         <v>21</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="24"/>
+      <c r="C28" s="54"/>
       <c r="D28" s="5" t="s">
         <v>47</v>
       </c>
       <c r="E28" s="6">
-        <v>2528000</v>
-      </c>
-      <c r="F28" s="15">
+        <v>2528</v>
+      </c>
+      <c r="F28" s="14">
         <v>600</v>
       </c>
-      <c r="J28" s="8">
-        <v>17251</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" ht="28.5" customHeight="1">
       <c r="A29" s="4">
         <v>22</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
       <c r="D29" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E29" s="6">
-        <v>1374240</v>
-      </c>
-      <c r="F29" s="15">
+        <v>1374.24</v>
+      </c>
+      <c r="F29" s="14">
         <v>420</v>
       </c>
-      <c r="J29" s="8">
-        <v>11830</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" ht="19">
       <c r="A30" s="4">
         <v>23</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
       <c r="D30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="6">
-        <v>594000</v>
-      </c>
-      <c r="F30" s="15">
+        <v>594</v>
+      </c>
+      <c r="F30" s="14">
         <v>123</v>
       </c>
-      <c r="J30" s="8">
-        <v>8600</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" ht="38">
       <c r="A31" s="4">
         <v>24</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="58"/>
       <c r="D31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="6">
-        <v>562500</v>
-      </c>
-      <c r="F31" s="15">
+        <v>562.5</v>
+      </c>
+      <c r="F31" s="14">
         <v>1394</v>
       </c>
-      <c r="J31" s="8">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" ht="19">
       <c r="A32" s="4">
         <v>25</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="58"/>
       <c r="D32" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E32" s="6">
-        <v>314100</v>
-      </c>
-      <c r="F32" s="15">
+        <v>314.10000000000002</v>
+      </c>
+      <c r="F32" s="14">
         <v>100</v>
       </c>
-      <c r="J32" s="8">
-        <v>6993</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" ht="28.5" customHeight="1">
       <c r="A33" s="4">
         <v>26</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="58"/>
       <c r="D33" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E33" s="6">
-        <v>503100</v>
-      </c>
-      <c r="F33" s="15">
+        <v>503.1</v>
+      </c>
+      <c r="F33" s="14">
         <v>45</v>
       </c>
-      <c r="J33" s="8">
-        <v>2250</v>
-      </c>
-      <c r="K33" s="50"/>
-    </row>
-    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J33" s="7"/>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="34" spans="1:11" ht="19">
       <c r="A34" s="4">
         <v>27</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="6">
-        <v>503000</v>
-      </c>
-      <c r="F34" s="15">
+        <v>503</v>
+      </c>
+      <c r="F34" s="14">
         <v>248</v>
       </c>
-      <c r="J34" s="67">
-        <f>SUM(J26:J33)</f>
-        <v>146440</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="J34" s="46"/>
+    </row>
+    <row r="35" spans="1:11" ht="19">
       <c r="A35" s="4">
         <v>28</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="58"/>
       <c r="D35" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E35" s="6">
-        <v>231525</v>
-      </c>
-      <c r="F35" s="15">
+        <v>231.52500000000001</v>
+      </c>
+      <c r="F35" s="14">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="24.75" customHeight="1">
       <c r="A36" s="4">
         <v>29</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="28"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
       <c r="D36" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E36" s="6">
-        <v>200000</v>
-      </c>
-      <c r="F36" s="15">
+        <v>200</v>
+      </c>
+      <c r="F36" s="14">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="19">
       <c r="A37" s="4">
         <v>30</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="6">
-        <v>182745</v>
-      </c>
-      <c r="F37" s="15">
+        <v>182.745</v>
+      </c>
+      <c r="F37" s="14">
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="24">
       <c r="A38" s="4"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="50">
-        <f>SUM(E28:E37)</f>
-        <v>6993210</v>
-      </c>
-      <c r="F38" s="52"/>
-    </row>
-    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12">
+      <c r="E38" s="6">
+        <v>6993.21</v>
+      </c>
+      <c r="F38" s="31"/>
+    </row>
+    <row r="39" spans="1:11" ht="21" customHeight="1">
+      <c r="A39" s="11">
         <v>31</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1774,14 +1787,14 @@
         <v>1</v>
       </c>
       <c r="E39" s="6">
-        <v>1250000</v>
-      </c>
-      <c r="F39" s="15">
+        <v>1250</v>
+      </c>
+      <c r="F39" s="14">
         <v>400</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A40" s="12">
+    <row r="40" spans="1:11" ht="38">
+      <c r="A40" s="11">
         <v>32</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1792,46 +1805,46 @@
         <v>38</v>
       </c>
       <c r="E40" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="F40" s="15">
+        <v>1000</v>
+      </c>
+      <c r="F40" s="14">
         <v>1200</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="55"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58" t="s">
+    <row r="41" spans="1:11" ht="24">
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="50">
+      <c r="E41" s="29">
         <f>SUM(E39:E40)</f>
-        <v>2250000</v>
-      </c>
-      <c r="F41" s="52"/>
-    </row>
-    <row r="42" spans="1:11" s="65" customFormat="1" ht="26.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F41" s="31"/>
+    </row>
+    <row r="42" spans="1:11" s="44" customFormat="1" ht="26">
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="63">
+      <c r="E42" s="42">
         <f>SUM(E41,E38,E27,E24,E21,E14,E8,E5)</f>
-        <v>146440530</v>
-      </c>
-      <c r="F42" s="64"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+        <v>146440.53</v>
+      </c>
+      <c r="F42" s="43"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>